<commit_message>
Updated TPS Screen Project
Added 4/28/2018 Info
</commit_message>
<xml_diff>
--- a/TPS Screen Project.xlsx
+++ b/TPS Screen Project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonah/Documents/ScreenManager/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCD8469-B53A-3249-BBC6-4C274603DFE5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72DC680-F4C2-4F44-9E54-D0A8882E4756}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9280" yWindow="440" windowWidth="16320" windowHeight="15560" xr2:uid="{B3020F1F-7DBC-E94A-AD1F-03F85764C2F4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{B3020F1F-7DBC-E94A-AD1F-03F85764C2F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>Task</t>
   </si>
@@ -76,13 +76,28 @@
   </si>
   <si>
     <t>Date: 04/21/2018</t>
+  </si>
+  <si>
+    <t>Date: 04/28/2018</t>
+  </si>
+  <si>
+    <t>Get touch keyboard to work with browser</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Test embedded browser</t>
+  </si>
+  <si>
+    <t>Jonah/Matt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -171,14 +186,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,35 +508,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5B692B-C8BC-674A-9507-E29D629E0114}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" customWidth="1"/>
-    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="1" max="1" width="53" customWidth="1"/>
+    <col min="2" max="2" width="14.125" customWidth="1"/>
+    <col min="3" max="3" width="6.625" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.625" customWidth="1"/>
+    <col min="7" max="7" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" ht="19">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -530,18 +547,18 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="19">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="19">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -564,30 +581,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="19">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>20</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>4</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>22</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <v>0.9</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="19">
+    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -603,14 +620,14 @@
       <c r="E6" s="3">
         <v>2</v>
       </c>
-      <c r="F6" s="3">
-        <v>10</v>
+      <c r="F6" s="5">
+        <v>0.1</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="19">
+    <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -626,17 +643,142 @@
       <c r="E7" s="3">
         <v>1</v>
       </c>
-      <c r="F7" s="3">
-        <v>10</v>
+      <c r="F7" s="5">
+        <v>0.1</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="4">
+        <v>4</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="5">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="3">
+        <v>6</v>
+      </c>
+      <c r="C16" s="3">
+        <v>4</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="3">
+        <v>3</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="3">
+        <v>10</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="3">
+        <v>5</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A13:G13"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>